<commit_message>
changed testfiles to relative paths
</commit_message>
<xml_diff>
--- a/test_files/test_schedule_1_mock_badDtypes.xlsx
+++ b/test_files/test_schedule_1_mock_badDtypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.mitter\Documents\streamscheduler\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B28A465-D677-4CBC-A68B-6DBF6624C270}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311284B0-BBF9-4F37-B6AF-7BADBF3A7595}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,13 +50,13 @@
     <t>dclive_0_1@2345</t>
   </si>
   <si>
-    <t>C:\Users\michael.mitter\Documents\streamscheduler\test_files\vids\test.mp4</t>
-  </si>
-  <si>
-    <t>C:\Users\michael.mitter\Documents\streamscheduler\test_files\vids\test2.mp4</t>
-  </si>
-  <si>
-    <t>C:\Users\michael.mitter\Documents\streamscheduler\test_files\vids\test4.mp4</t>
+    <t>test_files\vids\test.mp4</t>
+  </si>
+  <si>
+    <t>test_files\vids\test2.mp4</t>
+  </si>
+  <si>
+    <t>test_files\vids\test4.mp4</t>
   </si>
 </sst>
 </file>
@@ -913,7 +913,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
changed path to linux verions
</commit_message>
<xml_diff>
--- a/test_files/test_schedule_1_mock_badDtypes.xlsx
+++ b/test_files/test_schedule_1_mock_badDtypes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.mitter\Documents\streamscheduler\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311284B0-BBF9-4F37-B6AF-7BADBF3A7595}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69E915E-ED95-4686-B47E-AB800056B47E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,13 +50,13 @@
     <t>dclive_0_1@2345</t>
   </si>
   <si>
-    <t>test_files\vids\test.mp4</t>
-  </si>
-  <si>
-    <t>test_files\vids\test2.mp4</t>
-  </si>
-  <si>
-    <t>test_files\vids\test4.mp4</t>
+    <t>test_files/vids/test.mp4</t>
+  </si>
+  <si>
+    <t>test_files/vids/test2.mp4</t>
+  </si>
+  <si>
+    <t>test_files/vids/test4.mp4</t>
   </si>
 </sst>
 </file>
@@ -913,7 +913,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>